<commit_message>
Meer plaatjes, en vergelijking van bakjes
</commit_message>
<xml_diff>
--- a/bakjesExtrapoleren.xlsx
+++ b/bakjesExtrapoleren.xlsx
@@ -15744,8 +15744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
beetje getest met waar de 0 zit
</commit_message>
<xml_diff>
--- a/bakjesExtrapoleren.xlsx
+++ b/bakjesExtrapoleren.xlsx
@@ -7908,6 +7908,26 @@
                   <c:y val="-0.40152012248468943"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 9,8357e</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>-0,851x</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -26318,7 +26338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P208" workbookViewId="0">
       <selection activeCell="W227" sqref="W227"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
wat plaatjes voor de zekerheid
</commit_message>
<xml_diff>
--- a/bakjesExtrapoleren.xlsx
+++ b/bakjesExtrapoleren.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
   <si>
     <t>deltaCO2</t>
   </si>
@@ -139,7 +139,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -224,7 +223,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.5135608048993882E-3"/>
+                  <c:x val="-3.5135608048993887E-3"/>
                   <c:y val="-0.3314953339165938"/>
                 </c:manualLayout>
               </c:layout>
@@ -306,12 +305,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="77447552"/>
-        <c:axId val="77449088"/>
+        <c:axId val="64356352"/>
+        <c:axId val="64357888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77447552"/>
+        <c:axId val="64356352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,12 +364,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77449088"/>
+        <c:crossAx val="64357888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77449088"/>
+        <c:axId val="64357888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +424,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77447552"/>
+        <c:crossAx val="64356352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -468,7 +466,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -562,8 +560,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.5665135608049001E-2"/>
-                  <c:y val="-0.38804024496937889"/>
+                  <c:x val="-3.5665135608049008E-2"/>
+                  <c:y val="-0.38804024496937894"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -654,12 +652,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80447744"/>
-        <c:axId val="80461824"/>
+        <c:axId val="66619264"/>
+        <c:axId val="66620800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80447744"/>
+        <c:axId val="66619264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -714,12 +711,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80461824"/>
+        <c:crossAx val="66620800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80461824"/>
+        <c:axId val="66620800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -774,7 +771,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80447744"/>
+        <c:crossAx val="66619264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -816,7 +813,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -827,7 +824,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -993,12 +989,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80573184"/>
-        <c:axId val="80574720"/>
+        <c:axId val="66675072"/>
+        <c:axId val="66676608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80573184"/>
+        <c:axId val="66675072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1053,12 +1048,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80574720"/>
+        <c:crossAx val="66676608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80574720"/>
+        <c:axId val="66676608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1108,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80573184"/>
+        <c:crossAx val="66675072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1155,7 +1150,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1249,7 +1244,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.5891076115485566E-2"/>
+                  <c:x val="-1.589107611548557E-2"/>
                   <c:y val="-0.26304024496937883"/>
                 </c:manualLayout>
               </c:layout>
@@ -1331,12 +1326,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80608256"/>
-        <c:axId val="80614144"/>
+        <c:axId val="66701952"/>
+        <c:axId val="66707840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80608256"/>
+        <c:axId val="66701952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,12 +1385,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80614144"/>
+        <c:crossAx val="66707840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80614144"/>
+        <c:axId val="66707840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,7 +1445,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80608256"/>
+        <c:crossAx val="66701952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1493,7 +1487,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1589,7 +1583,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="2.5886701662292209E-2"/>
-                  <c:y val="-0.29081802274715668"/>
+                  <c:y val="-0.29081802274715673"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -1674,12 +1668,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80672256"/>
-        <c:axId val="80673792"/>
+        <c:axId val="66823296"/>
+        <c:axId val="66824832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80672256"/>
+        <c:axId val="66823296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1734,12 +1727,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80673792"/>
+        <c:crossAx val="66824832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80673792"/>
+        <c:axId val="66824832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1794,7 +1787,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80672256"/>
+        <c:crossAx val="66823296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1836,7 +1829,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1930,8 +1923,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.1004811898512699E-2"/>
-                  <c:y val="-0.39258821813939937"/>
+                  <c:x val="-5.1004811898512706E-2"/>
+                  <c:y val="-0.39258821813939943"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -2022,12 +2015,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80707584"/>
-        <c:axId val="80709120"/>
+        <c:axId val="68173184"/>
+        <c:axId val="68203648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80707584"/>
+        <c:axId val="68173184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2082,12 +2074,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80709120"/>
+        <c:crossAx val="68203648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80709120"/>
+        <c:axId val="68203648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2142,7 +2134,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80707584"/>
+        <c:crossAx val="68173184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2184,7 +2176,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2360,12 +2352,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80828672"/>
-        <c:axId val="80830464"/>
+        <c:axId val="68310912"/>
+        <c:axId val="68312448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80828672"/>
+        <c:axId val="68310912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2420,12 +2411,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80830464"/>
+        <c:crossAx val="68312448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80830464"/>
+        <c:axId val="68312448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,7 +2471,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80828672"/>
+        <c:crossAx val="68310912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2522,7 +2513,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2617,7 +2608,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-4.6688538932633424E-3"/>
-                  <c:y val="-0.34637357830271226"/>
+                  <c:y val="-0.34637357830271237"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2692,12 +2683,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80745600"/>
-        <c:axId val="80845824"/>
+        <c:axId val="68231552"/>
+        <c:axId val="68233088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80745600"/>
+        <c:axId val="68231552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2752,12 +2742,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80845824"/>
+        <c:crossAx val="68233088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80845824"/>
+        <c:axId val="68233088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2812,7 +2802,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80745600"/>
+        <c:crossAx val="68231552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2854,7 +2844,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2865,7 +2855,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2949,7 +2938,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.4554024496937877E-2"/>
+                  <c:x val="-2.4554024496937873E-2"/>
                   <c:y val="-0.24915135608048994"/>
                 </c:manualLayout>
               </c:layout>
@@ -3043,12 +3032,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80641024"/>
-        <c:axId val="80773888"/>
+        <c:axId val="68258432"/>
+        <c:axId val="68260224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80641024"/>
+        <c:axId val="68258432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3103,12 +3091,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80773888"/>
+        <c:crossAx val="68260224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80773888"/>
+        <c:axId val="68260224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3163,7 +3151,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80641024"/>
+        <c:crossAx val="68258432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3205,7 +3193,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3216,7 +3204,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3357,12 +3344,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80950784"/>
-        <c:axId val="80952320"/>
+        <c:axId val="68703360"/>
+        <c:axId val="68704896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80950784"/>
+        <c:axId val="68703360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3417,12 +3403,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80952320"/>
+        <c:crossAx val="68704896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80952320"/>
+        <c:axId val="68704896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3477,7 +3463,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80950784"/>
+        <c:crossAx val="68703360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3519,7 +3505,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3530,7 +3516,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3659,12 +3644,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80997376"/>
-        <c:axId val="80888576"/>
+        <c:axId val="68733568"/>
+        <c:axId val="68362624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80997376"/>
+        <c:axId val="68733568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3719,12 +3703,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80888576"/>
+        <c:crossAx val="68362624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80888576"/>
+        <c:axId val="68362624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3779,7 +3763,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80997376"/>
+        <c:crossAx val="68733568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3821,7 +3805,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3916,7 +3900,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.5375328083989507E-2"/>
+                  <c:x val="3.5375328083989521E-2"/>
                   <c:y val="-0.26669473607465732"/>
                 </c:manualLayout>
               </c:layout>
@@ -3998,12 +3982,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="75315840"/>
-        <c:axId val="75329920"/>
+        <c:axId val="64375040"/>
+        <c:axId val="64380928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75315840"/>
+        <c:axId val="64375040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4058,12 +4041,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75329920"/>
+        <c:crossAx val="64380928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75329920"/>
+        <c:axId val="64380928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4118,7 +4101,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75315840"/>
+        <c:crossAx val="64375040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4160,7 +4143,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4171,7 +4154,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4306,12 +4288,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80913920"/>
-        <c:axId val="80915456"/>
+        <c:axId val="68404352"/>
+        <c:axId val="68405888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80913920"/>
+        <c:axId val="68404352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4366,12 +4347,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80915456"/>
+        <c:crossAx val="68405888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80915456"/>
+        <c:axId val="68405888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4426,7 +4407,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80913920"/>
+        <c:crossAx val="68404352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4468,7 +4449,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4479,7 +4460,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4564,7 +4544,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-9.1220691163604567E-2"/>
-                  <c:y val="-0.19822543015456404"/>
+                  <c:y val="-0.19822543015456406"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4645,12 +4625,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81043840"/>
-        <c:axId val="81045376"/>
+        <c:axId val="68792320"/>
+        <c:axId val="68793856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81043840"/>
+        <c:axId val="68792320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4705,12 +4684,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81045376"/>
+        <c:crossAx val="68793856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81045376"/>
+        <c:axId val="68793856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4765,7 +4744,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81043840"/>
+        <c:crossAx val="68792320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4807,7 +4786,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4818,7 +4797,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4904,8 +4882,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.3439632545931778E-2"/>
-                  <c:y val="-0.29894757946923306"/>
+                  <c:x val="4.3439632545931792E-2"/>
+                  <c:y val="-0.29894757946923312"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4986,12 +4964,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81140352"/>
-        <c:axId val="81162624"/>
+        <c:axId val="68888832"/>
+        <c:axId val="68898816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81140352"/>
+        <c:axId val="68888832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5046,12 +5023,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81162624"/>
+        <c:crossAx val="68898816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81162624"/>
+        <c:axId val="68898816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5106,7 +5083,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81140352"/>
+        <c:crossAx val="68888832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5148,7 +5125,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5159,7 +5136,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5243,8 +5219,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.089370078740159E-2"/>
-                  <c:y val="-0.34685367454068244"/>
+                  <c:x val="-6.0893700787401597E-2"/>
+                  <c:y val="-0.3468536745406825"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5319,12 +5295,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81179776"/>
-        <c:axId val="81181312"/>
+        <c:axId val="68928256"/>
+        <c:axId val="68929792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81179776"/>
+        <c:axId val="68928256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5379,12 +5354,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81181312"/>
+        <c:crossAx val="68929792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81181312"/>
+        <c:axId val="68929792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5439,7 +5414,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81179776"/>
+        <c:crossAx val="68928256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5481,7 +5456,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5492,7 +5467,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5576,8 +5550,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.1078873578302712"/>
-                  <c:y val="-0.35100320793234185"/>
+                  <c:x val="-0.10788735783027119"/>
+                  <c:y val="-0.35100320793234191"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -5680,12 +5654,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81120640"/>
-        <c:axId val="81204352"/>
+        <c:axId val="68844544"/>
+        <c:axId val="68948736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81120640"/>
+        <c:axId val="68844544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5740,12 +5713,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81204352"/>
+        <c:crossAx val="68948736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81204352"/>
+        <c:axId val="68948736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5800,7 +5773,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81120640"/>
+        <c:crossAx val="68844544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5842,7 +5815,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5853,7 +5826,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5937,8 +5909,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.10933814523184604"/>
-                  <c:y val="-0.3250703557888599"/>
+                  <c:x val="-0.10933814523184605"/>
+                  <c:y val="-0.32507035578886001"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -6041,12 +6013,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81237504"/>
-        <c:axId val="81239040"/>
+        <c:axId val="68985984"/>
+        <c:axId val="68987520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81237504"/>
+        <c:axId val="68985984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6101,12 +6072,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81239040"/>
+        <c:crossAx val="68987520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81239040"/>
+        <c:axId val="68987520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6161,7 +6132,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81237504"/>
+        <c:crossAx val="68985984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6203,7 +6174,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6338,12 +6309,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81297408"/>
-        <c:axId val="81298944"/>
+        <c:axId val="69549440"/>
+        <c:axId val="69571712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81297408"/>
+        <c:axId val="69549440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6398,12 +6368,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81298944"/>
+        <c:crossAx val="69571712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81298944"/>
+        <c:axId val="69571712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6458,7 +6428,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81297408"/>
+        <c:crossAx val="69549440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6500,7 +6470,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6736,12 +6706,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="81231232"/>
-        <c:axId val="81339520"/>
+        <c:axId val="68975616"/>
+        <c:axId val="69604096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="81231232"/>
+        <c:axId val="68975616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6796,12 +6765,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81339520"/>
+        <c:crossAx val="69604096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81339520"/>
+        <c:axId val="69604096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6856,7 +6825,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81231232"/>
+        <c:crossAx val="68975616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6929,7 +6898,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6971,8 +6940,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.3450568678915135E-2"/>
-                  <c:y val="-0.3969597550306212"/>
+                  <c:x val="-1.3450568678915139E-2"/>
+                  <c:y val="-0.39695975503062131"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -7047,23 +7016,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="86209280"/>
-        <c:axId val="85052416"/>
+        <c:axId val="69623808"/>
+        <c:axId val="69625344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86209280"/>
+        <c:axId val="69623808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85052416"/>
+        <c:crossAx val="69625344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85052416"/>
+        <c:axId val="69625344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7071,7 +7040,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86209280"/>
+        <c:crossAx val="69623808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7084,7 +7053,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7126,8 +7095,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.6378390201224845E-2"/>
-                  <c:y val="-0.40621901428988044"/>
+                  <c:x val="-1.6378390201224842E-2"/>
+                  <c:y val="-0.4062190142898805"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -7202,23 +7171,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101949824"/>
-        <c:axId val="101939840"/>
+        <c:axId val="69736320"/>
+        <c:axId val="69737856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101949824"/>
+        <c:axId val="69736320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101939840"/>
+        <c:crossAx val="69737856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="101939840"/>
+        <c:axId val="69737856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7226,7 +7195,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101949824"/>
+        <c:crossAx val="69736320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7239,7 +7208,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7384,12 +7353,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="77403264"/>
-        <c:axId val="77404800"/>
+        <c:axId val="64570112"/>
+        <c:axId val="64571648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77403264"/>
+        <c:axId val="64570112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7444,12 +7412,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77404800"/>
+        <c:crossAx val="64571648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77404800"/>
+        <c:axId val="64571648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7504,7 +7472,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77403264"/>
+        <c:crossAx val="64570112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7546,7 +7514,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7588,8 +7556,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-5.7895888013998246E-4"/>
-                  <c:y val="-0.39082567804024498"/>
+                  <c:x val="-5.7895888013998267E-4"/>
+                  <c:y val="-0.39082567804024509"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -7664,23 +7632,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="69255552"/>
-        <c:axId val="69253760"/>
+        <c:axId val="69779456"/>
+        <c:axId val="69780992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69255552"/>
+        <c:axId val="69779456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69253760"/>
+        <c:crossAx val="69780992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69253760"/>
+        <c:axId val="69780992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7688,7 +7656,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69255552"/>
+        <c:crossAx val="69779456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7701,7 +7669,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7744,7 +7712,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-4.0630139982502186E-2"/>
-                  <c:y val="-0.33214494021580637"/>
+                  <c:y val="-0.33214494021580643"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -7825,23 +7793,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="83576320"/>
-        <c:axId val="83574784"/>
+        <c:axId val="62986112"/>
+        <c:axId val="62987648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83576320"/>
+        <c:axId val="62986112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83574784"/>
+        <c:crossAx val="62987648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83574784"/>
+        <c:axId val="62987648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7849,7 +7817,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83576320"/>
+        <c:crossAx val="62986112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7862,7 +7830,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7904,8 +7872,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.1716972878390202E-2"/>
-                  <c:y val="-0.40152012248468943"/>
+                  <c:x val="1.17169728783902E-2"/>
+                  <c:y val="-0.40152012248468949"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -7986,23 +7954,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="90362624"/>
-        <c:axId val="89039616"/>
+        <c:axId val="63032704"/>
+        <c:axId val="63038592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90362624"/>
+        <c:axId val="63032704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89039616"/>
+        <c:crossAx val="63038592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="89039616"/>
+        <c:axId val="63038592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8010,7 +7978,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90362624"/>
+        <c:crossAx val="63032704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8023,7 +7991,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8194,12 +8162,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="77917568"/>
-        <c:axId val="80159872"/>
+        <c:axId val="64609280"/>
+        <c:axId val="66065152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77917568"/>
+        <c:axId val="64609280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8254,12 +8221,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80159872"/>
+        <c:crossAx val="66065152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80159872"/>
+        <c:axId val="66065152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8314,7 +8281,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77917568"/>
+        <c:crossAx val="64609280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8356,7 +8323,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8367,7 +8334,6 @@
   <c:lang val="nl-NL"/>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -8545,12 +8511,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80193408"/>
-        <c:axId val="80194944"/>
+        <c:axId val="66086400"/>
+        <c:axId val="66087936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80193408"/>
+        <c:axId val="66086400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8605,12 +8570,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80194944"/>
+        <c:crossAx val="66087936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80194944"/>
+        <c:axId val="66087936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8665,7 +8630,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80193408"/>
+        <c:crossAx val="66086400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8707,7 +8672,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8870,12 +8835,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80286848"/>
-        <c:axId val="80288384"/>
+        <c:axId val="66208512"/>
+        <c:axId val="66210048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80286848"/>
+        <c:axId val="66208512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8930,12 +8894,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80288384"/>
+        <c:crossAx val="66210048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80288384"/>
+        <c:axId val="66210048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8990,7 +8954,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80286848"/>
+        <c:crossAx val="66208512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9032,7 +8996,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9127,7 +9091,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="1.7553368328958881E-2"/>
-                  <c:y val="-0.29081802274715668"/>
+                  <c:y val="-0.29081802274715673"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -9230,12 +9194,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80371072"/>
-        <c:axId val="80376960"/>
+        <c:axId val="66280448"/>
+        <c:axId val="66294528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80371072"/>
+        <c:axId val="66280448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9290,12 +9253,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80376960"/>
+        <c:crossAx val="66294528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80376960"/>
+        <c:axId val="66294528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9350,7 +9313,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80371072"/>
+        <c:crossAx val="66280448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9392,7 +9355,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9486,8 +9449,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.8829177602799653E-2"/>
-                  <c:y val="-0.34637357830271226"/>
+                  <c:x val="-1.8829177602799656E-2"/>
+                  <c:y val="-0.34637357830271237"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -9574,12 +9537,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80406400"/>
-        <c:axId val="80407936"/>
+        <c:axId val="66315776"/>
+        <c:axId val="66317312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80406400"/>
+        <c:axId val="66315776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9634,12 +9596,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80407936"/>
+        <c:crossAx val="66317312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80407936"/>
+        <c:axId val="66317312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9694,7 +9656,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80406400"/>
+        <c:crossAx val="66315776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9736,7 +9698,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9831,7 +9793,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-6.224409448818898E-3"/>
-                  <c:y val="-0.4435958005249343"/>
+                  <c:y val="-0.44359580052493425"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -9928,12 +9890,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="80277504"/>
-        <c:axId val="80279040"/>
+        <c:axId val="66174336"/>
+        <c:axId val="66184320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80277504"/>
+        <c:axId val="66174336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9988,12 +9949,12 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80279040"/>
+        <c:crossAx val="66184320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80279040"/>
+        <c:axId val="66184320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10048,7 +10009,7 @@
             <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80277504"/>
+        <c:crossAx val="66174336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10090,7 +10051,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -26328,7 +26289,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -26336,10 +26297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC224"/>
+  <dimension ref="A1:AC221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P208" workbookViewId="0">
-      <selection activeCell="W227" sqref="W227"/>
+    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
+      <selection activeCell="D226" sqref="D226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27353,121 +27314,13 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="218" spans="1:6">
-      <c r="A218" t="s">
-        <v>0</v>
-      </c>
-      <c r="B218" t="s">
-        <v>1</v>
-      </c>
-      <c r="C218" t="s">
-        <v>2</v>
-      </c>
-      <c r="D218" t="s">
-        <v>3</v>
-      </c>
-      <c r="F218" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="219" spans="1:6">
-      <c r="A219">
-        <v>0.686164</v>
-      </c>
-      <c r="B219">
-        <v>1.7387779999999999</v>
-      </c>
-      <c r="C219">
-        <v>0.69276470000000001</v>
-      </c>
-      <c r="D219" s="4">
-        <f>9.1525*EXP(-0.823*A219)</f>
-        <v>5.2034095531144695</v>
-      </c>
-      <c r="F219">
-        <f>(B219-C219)/(D219-C219)</f>
-        <v>0.23189883798494088</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6">
-      <c r="A220">
-        <v>1.313366</v>
-      </c>
-      <c r="B220">
-        <v>1</v>
-      </c>
-      <c r="C220">
-        <v>0.30195050000000001</v>
-      </c>
-      <c r="D220">
-        <v>3.5077959999999999</v>
-      </c>
-      <c r="F220">
-        <f t="shared" ref="F220:F223" si="4">(B220-C220)/(D220-C220)</f>
-        <v>0.21774271405156614</v>
-      </c>
+      <c r="D219" s="4"/>
     </row>
     <row r="221" spans="1:6">
-      <c r="A221">
-        <v>2.1761309999999998</v>
-      </c>
-      <c r="B221" s="4">
-        <v>0.5667325029055762</v>
-      </c>
-      <c r="C221" s="4">
-        <f>2.1434*EXP(-1.378*A221)</f>
-        <v>0.10685151006976371</v>
-      </c>
-      <c r="D221" s="4">
-        <f>9.1525*EXP(-0.823*A221)</f>
-        <v>1.5266430700085469</v>
-      </c>
-      <c r="F221">
-        <f t="shared" si="4"/>
-        <v>0.3239074000803619</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6">
-      <c r="A222">
-        <v>2.9109790000000002</v>
-      </c>
-      <c r="B222">
-        <v>0.2418014</v>
-      </c>
-      <c r="C222">
-        <v>7.4589890000000006E-2</v>
-      </c>
-      <c r="D222">
-        <v>1.116473</v>
-      </c>
-      <c r="F222">
-        <f t="shared" si="4"/>
-        <v>0.16048970215094474</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6">
-      <c r="A223">
-        <v>4.1693759999999997</v>
-      </c>
-      <c r="B223">
-        <v>0.1883726</v>
-      </c>
-      <c r="C223">
-        <v>1.2652679999999999E-2</v>
-      </c>
-      <c r="D223">
-        <v>0.67469699999999999</v>
-      </c>
-      <c r="F223">
-        <f t="shared" si="4"/>
-        <v>0.26542017609938862</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6">
-      <c r="F224">
-        <f>AVERAGE(F219:F223)</f>
-        <v>0.23989176607344045</v>
-      </c>
+      <c r="B221" s="4"/>
+      <c r="C221" s="4"/>
+      <c r="D221" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>